<commit_message>
add ET message reset function
</commit_message>
<xml_diff>
--- a/Design/Excel/ET/Datas/__beans__.xlsx
+++ b/Design/Excel/ET/Datas/__beans__.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22331" windowHeight="8484"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>##var</t>
   </si>
@@ -68,117 +68,6 @@
   </si>
   <si>
     <t>注释</t>
-  </si>
-  <si>
-    <t>item.ItemExchange</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>道具id</t>
-  </si>
-  <si>
-    <t>num</t>
-  </si>
-  <si>
-    <t>道具数量</t>
-  </si>
-  <si>
-    <t>test.TestExcelBean1</t>
-  </si>
-  <si>
-    <t>这是个测试excel结构</t>
-  </si>
-  <si>
-    <t>x1</t>
-  </si>
-  <si>
-    <t>最高品质</t>
-  </si>
-  <si>
-    <t>x2</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>黑色的</t>
-  </si>
-  <si>
-    <t>x3</t>
-  </si>
-  <si>
-    <t>蓝色的</t>
-  </si>
-  <si>
-    <t>x4</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>最差品质</t>
-  </si>
-  <si>
-    <t>test.TestExcelBean2</t>
-  </si>
-  <si>
-    <t>y1</t>
-  </si>
-  <si>
-    <t>y2</t>
-  </si>
-  <si>
-    <t>y3</t>
-  </si>
-  <si>
-    <t>test.Shape</t>
-  </si>
-  <si>
-    <t>test.Circle</t>
-  </si>
-  <si>
-    <t>Shape</t>
-  </si>
-  <si>
-    <t>圆</t>
-  </si>
-  <si>
-    <t>这是一个圆</t>
-  </si>
-  <si>
-    <t>radius</t>
-  </si>
-  <si>
-    <t>半径</t>
-  </si>
-  <si>
-    <t>test.Rectangle</t>
-  </si>
-  <si>
-    <t>矩形</t>
-  </si>
-  <si>
-    <t>这是一个矩形</t>
-  </si>
-  <si>
-    <t>width</t>
-  </si>
-  <si>
-    <t>宽度</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>高度</t>
   </si>
 </sst>
 </file>
@@ -191,7 +80,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,20 +98,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -666,10 +541,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -678,7 +553,7 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -687,124 +562,124 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -818,10 +693,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="31" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1146,16 +1021,16 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="3" width="20.6296296296296" customWidth="1"/>
+    <col min="2" max="3" width="20.6333333333333" customWidth="1"/>
     <col min="4" max="5" width="12.25" customWidth="1"/>
     <col min="6" max="7" width="15" customWidth="1"/>
     <col min="8" max="9" width="13.5" customWidth="1"/>
-    <col min="10" max="10" width="10.3796296296296" customWidth="1"/>
+    <col min="10" max="10" width="10.3833333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1232,127 +1107,23 @@
       </c>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="H4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="8:11">
-      <c r="H5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="8:11">
-      <c r="H7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="8:11">
-      <c r="H8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="8:11">
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="8:11">
-      <c r="H11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="8:11">
-      <c r="H12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" t="s">
-        <v>33</v>
-      </c>
+    <row r="6" spans="2:2">
+      <c r="B6" s="3"/>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1364,56 +1135,28 @@
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" s="4"/>
@@ -1422,16 +1165,10 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="K16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>